<commit_message>
sửa lại thống kê, cập nhật danh sách sv trước tốt nghiệp
</commit_message>
<xml_diff>
--- a/nuce.web.api/Templates/Survey/MauUploadTruocTotNghiep.xlsx
+++ b/nuce.web.api/Templates/Survey/MauUploadTruocTotNghiep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\nuce.web\nuce.web.api\Templates\Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB6159D-C835-4848-AC22-287AF054E3FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27C05B6-E6E2-4DB8-9AD4-961E59978E11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>STT</t>
   </si>
@@ -64,13 +64,16 @@
   </si>
   <si>
     <t>Tên ngành</t>
+  </si>
+  <si>
+    <t>Ngày ra quyết định</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,38 +89,46 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val=".VnTime"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val=".VnTime"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val=".VnTime"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val=".VnTime"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,36 +175,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -476,103 +496,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C4" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="22" style="8" customWidth="1"/>
-    <col min="3" max="3" width="30" style="8" customWidth="1"/>
-    <col min="4" max="4" width="18.375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9" style="8"/>
-    <col min="8" max="9" width="16.875" style="8" customWidth="1"/>
-    <col min="10" max="10" width="26.625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="8" customWidth="1"/>
-    <col min="12" max="12" width="16" style="8" customWidth="1"/>
-    <col min="13" max="13" width="48" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="8"/>
+    <col min="1" max="1" width="10.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9" style="3"/>
+    <col min="8" max="9" width="16.875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="26.625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" customWidth="1"/>
+    <col min="13" max="13" width="48" style="3" customWidth="1"/>
+    <col min="14" max="14" width="21.875" style="12" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="53.25" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="N1" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="15">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="1"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="1"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="6"/>
     </row>
-    <row r="9" spans="1:13">
-      <c r="D9" s="9"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D9" s="8"/>
     </row>
-    <row r="11" spans="1:13">
-      <c r="C11" s="9"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>